<commit_message>
Driving all jury updates.
</commit_message>
<xml_diff>
--- a/src/main/resources/devices/biy/Jury.xlsx
+++ b/src/main/resources/devices/biy/Jury.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Dev\git\owlcms-firmata\src\main\resources\devices\biy\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{49B56EF4-61FA-4351-8B7C-8D162262C28C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{293838E6-1847-40E7-AF1A-827C96684CEA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-22560" yWindow="612" windowWidth="22416" windowHeight="11292" xr2:uid="{F9C8F068-60C0-4FDD-8C1E-880F519290ED}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{F9C8F068-60C0-4FDD-8C1E-880F519290ED}"/>
   </bookViews>
   <sheets>
     <sheet name="Jury" sheetId="2" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="327" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="449" uniqueCount="163">
   <si>
     <t>pin</t>
   </si>
@@ -394,6 +394,135 @@
   </si>
   <si>
     <t>5 bad</t>
+  </si>
+  <si>
+    <t>Jury 1 LED G Red</t>
+  </si>
+  <si>
+    <t>Jury 2 LED G Red</t>
+  </si>
+  <si>
+    <t>Jury 3 LED G Red</t>
+  </si>
+  <si>
+    <t>Jury 4 LED G Red</t>
+  </si>
+  <si>
+    <t>Jury 5 LED G Red</t>
+  </si>
+  <si>
+    <t>Jury 2 LED B Red</t>
+  </si>
+  <si>
+    <t>Jury 2 LED R Green</t>
+  </si>
+  <si>
+    <t>Jury 2 LED B Green</t>
+  </si>
+  <si>
+    <t>Jury 1 LED R Green</t>
+  </si>
+  <si>
+    <t>Jury 1 LED B Green</t>
+  </si>
+  <si>
+    <t>Jury 1 LED B Red</t>
+  </si>
+  <si>
+    <t>Jury 3 LED R Green</t>
+  </si>
+  <si>
+    <t>Jury 3 LED B Green</t>
+  </si>
+  <si>
+    <t>Jury 3 LED B Red</t>
+  </si>
+  <si>
+    <t>Jury 4 LED R Green</t>
+  </si>
+  <si>
+    <t>Jury 4 LED B Green</t>
+  </si>
+  <si>
+    <t>Jury 4 LED B Red</t>
+  </si>
+  <si>
+    <t>Jury 5 LED R Green</t>
+  </si>
+  <si>
+    <t>5 hidden</t>
+  </si>
+  <si>
+    <t>Jury 5 LED G Green</t>
+  </si>
+  <si>
+    <t>Jury 5 LED B Green</t>
+  </si>
+  <si>
+    <t>Jury 5 LED R Red</t>
+  </si>
+  <si>
+    <t>Jury 5 LED B Red</t>
+  </si>
+  <si>
+    <t>Jury 5 LED R White</t>
+  </si>
+  <si>
+    <t>Jury 5 LED G White</t>
+  </si>
+  <si>
+    <t>Jury 5 LED B White</t>
+  </si>
+  <si>
+    <t>Jury 5 LED R Off</t>
+  </si>
+  <si>
+    <t>Jury 5 LED G Off</t>
+  </si>
+  <si>
+    <t>Jury 5 LED B Off</t>
+  </si>
+  <si>
+    <t>Jury 5 Good</t>
+  </si>
+  <si>
+    <t>Jury 5 Bad</t>
+  </si>
+  <si>
+    <t>Ref 1 LED R startup test</t>
+  </si>
+  <si>
+    <t>Ref 1 LED B startup test</t>
+  </si>
+  <si>
+    <t>Ref 1 Bad G red</t>
+  </si>
+  <si>
+    <t>Ref 1 Bad B red</t>
+  </si>
+  <si>
+    <t>Ref 2 LED R startup test</t>
+  </si>
+  <si>
+    <t>Ref 2 LED B startup test</t>
+  </si>
+  <si>
+    <t>Ref 2 Bad G red</t>
+  </si>
+  <si>
+    <t>Ref 2 Bad B red</t>
+  </si>
+  <si>
+    <t>Ref 3 LED R startup test</t>
+  </si>
+  <si>
+    <t>Ref 3 LED B startup test</t>
+  </si>
+  <si>
+    <t>Ref 3 Bad G red</t>
+  </si>
+  <si>
+    <t>Ref 3 Bad B red</t>
   </si>
 </sst>
 </file>
@@ -439,12 +568,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor rgb="FFFFC000"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -452,6 +575,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -468,7 +597,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -477,9 +606,11 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -795,10 +926,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{068CC8FA-5BAB-452A-BED2-2AD75A3C9C5E}">
-  <dimension ref="A1:I91"/>
+  <dimension ref="A1:I123"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="J95" sqref="J95"/>
+    <sheetView tabSelected="1" topLeftCell="A37" workbookViewId="0">
+      <selection activeCell="B51" sqref="B51:B53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -809,7 +940,7 @@
     <col min="4" max="4" width="9" customWidth="1"/>
     <col min="5" max="5" width="10.85546875" style="3" customWidth="1"/>
     <col min="6" max="6" width="11.28515625" style="2" customWidth="1"/>
-    <col min="7" max="7" width="15.28515625" style="2" customWidth="1"/>
+    <col min="7" max="7" width="13.42578125" style="2" customWidth="1"/>
     <col min="8" max="8" width="24.140625" customWidth="1"/>
     <col min="9" max="9" width="14.140625" style="2" customWidth="1"/>
   </cols>
@@ -966,7 +1097,7 @@
       <c r="A9" t="s">
         <v>45</v>
       </c>
-      <c r="B9">
+      <c r="B9" s="5">
         <v>13</v>
       </c>
       <c r="C9" s="1" t="s">
@@ -980,7 +1111,7 @@
       <c r="A10" t="s">
         <v>46</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="5">
         <v>12</v>
       </c>
       <c r="C10" s="1" t="s">
@@ -994,7 +1125,7 @@
       <c r="A11" t="s">
         <v>47</v>
       </c>
-      <c r="B11">
+      <c r="B11" s="5">
         <v>11</v>
       </c>
       <c r="C11" s="1" t="s">
@@ -1006,17 +1137,16 @@
     </row>
     <row r="12" spans="1:9">
       <c r="A12" t="s">
-        <v>48</v>
-      </c>
-      <c r="B12" s="7">
-        <f>B10</f>
-        <v>12</v>
+        <v>151</v>
+      </c>
+      <c r="B12" s="5">
+        <v>13</v>
       </c>
       <c r="C12" t="s">
         <v>6</v>
       </c>
       <c r="E12" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="F12" s="2">
         <v>1000</v>
@@ -1024,53 +1154,50 @@
     </row>
     <row r="13" spans="1:9">
       <c r="A13" t="s">
-        <v>52</v>
-      </c>
-      <c r="B13" s="7">
-        <f>B9</f>
-        <v>13</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D13" t="s">
-        <v>10</v>
+        <v>48</v>
+      </c>
+      <c r="B13" s="5">
+        <v>12</v>
+      </c>
+      <c r="C13" t="s">
+        <v>6</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>3</v>
+      </c>
+      <c r="F13" s="2">
+        <v>1000</v>
       </c>
     </row>
     <row r="14" spans="1:9">
       <c r="A14" t="s">
-        <v>49</v>
-      </c>
-      <c r="B14" s="7">
-        <f>B9</f>
-        <v>13</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D14" t="s">
+        <v>152</v>
+      </c>
+      <c r="B14" s="5">
         <v>11</v>
       </c>
+      <c r="C14" t="s">
+        <v>6</v>
+      </c>
       <c r="E14" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
+      </c>
+      <c r="F14" s="2">
+        <v>1000</v>
       </c>
     </row>
     <row r="15" spans="1:9">
       <c r="A15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B15" s="7">
-        <f>B10</f>
-        <v>12</v>
+        <v>52</v>
+      </c>
+      <c r="B15" s="5">
+        <v>13</v>
       </c>
       <c r="C15" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D15" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>3</v>
@@ -1078,199 +1205,186 @@
     </row>
     <row r="16" spans="1:9">
       <c r="A16" t="s">
-        <v>51</v>
-      </c>
-      <c r="B16" s="7">
-        <f>B11</f>
-        <v>11</v>
+        <v>153</v>
+      </c>
+      <c r="B16" s="5">
+        <v>12</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D16" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:9">
       <c r="A17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B17">
+        <v>154</v>
+      </c>
+      <c r="B17" s="5">
+        <v>11</v>
+      </c>
+      <c r="C17" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" t="s">
         <v>10</v>
       </c>
-      <c r="C17" s="1"/>
-      <c r="G17" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H17" t="s">
-        <v>108</v>
-      </c>
-      <c r="I17" s="2">
-        <v>1</v>
+      <c r="E17" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="18" spans="1:9">
       <c r="A18" t="s">
-        <v>53</v>
-      </c>
-      <c r="B18">
-        <v>9</v>
+        <v>49</v>
+      </c>
+      <c r="B18" s="8">
+        <v>13</v>
       </c>
       <c r="C18" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
+      </c>
+      <c r="D18" t="s">
+        <v>11</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="19" spans="1:9">
       <c r="A19" t="s">
-        <v>54</v>
-      </c>
-      <c r="B19">
-        <v>8</v>
+        <v>50</v>
+      </c>
+      <c r="B19" s="8">
+        <v>12</v>
       </c>
       <c r="C19" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
+      </c>
+      <c r="D19" t="s">
+        <v>11</v>
       </c>
       <c r="E19" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="20" spans="1:9">
       <c r="A20" t="s">
-        <v>55</v>
-      </c>
-      <c r="B20">
-        <v>7</v>
+        <v>51</v>
+      </c>
+      <c r="B20" s="8">
+        <v>11</v>
       </c>
       <c r="C20" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
+      </c>
+      <c r="D20" t="s">
+        <v>11</v>
       </c>
       <c r="E20" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="21" spans="1:9">
       <c r="A21" t="s">
-        <v>56</v>
-      </c>
-      <c r="B21" s="7">
-        <f>B19</f>
-        <v>8</v>
-      </c>
-      <c r="C21" t="s">
-        <v>6</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F21" s="2">
-        <v>1000</v>
+        <v>25</v>
+      </c>
+      <c r="B21" s="9">
+        <v>10</v>
+      </c>
+      <c r="C21" s="1"/>
+      <c r="G21" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H21" t="s">
+        <v>108</v>
+      </c>
+      <c r="I21" s="2">
+        <v>1</v>
       </c>
     </row>
     <row r="22" spans="1:9">
       <c r="A22" t="s">
-        <v>57</v>
-      </c>
-      <c r="B22" s="7">
-        <f>B18</f>
+        <v>53</v>
+      </c>
+      <c r="B22" s="5">
         <v>9</v>
       </c>
       <c r="C22" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D22" t="s">
-        <v>42</v>
+        <v>4</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="23" spans="1:9">
       <c r="A23" t="s">
-        <v>58</v>
-      </c>
-      <c r="B23" s="7">
-        <f>B18</f>
-        <v>9</v>
+        <v>54</v>
+      </c>
+      <c r="B23" s="5">
+        <v>8</v>
       </c>
       <c r="C23" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D23" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:9">
       <c r="A24" t="s">
-        <v>59</v>
-      </c>
-      <c r="B24" s="7">
-        <f>B19</f>
-        <v>8</v>
+        <v>55</v>
+      </c>
+      <c r="B24" s="5">
+        <v>7</v>
       </c>
       <c r="C24" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D24" t="s">
-        <v>43</v>
+        <v>4</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="25" spans="1:9">
       <c r="A25" t="s">
-        <v>60</v>
-      </c>
-      <c r="B25" s="7">
-        <f>B20</f>
-        <v>7</v>
-      </c>
-      <c r="C25" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D25" t="s">
-        <v>43</v>
+        <v>155</v>
+      </c>
+      <c r="B25" s="5">
+        <v>9</v>
+      </c>
+      <c r="C25" t="s">
+        <v>6</v>
       </c>
       <c r="E25" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="26" spans="1:9">
       <c r="A26" t="s">
-        <v>44</v>
-      </c>
-      <c r="B26">
+        <v>56</v>
+      </c>
+      <c r="B26" s="5">
+        <v>8</v>
+      </c>
+      <c r="C26" t="s">
         <v>6</v>
       </c>
-      <c r="C26" s="1"/>
-      <c r="G26" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H26" t="s">
-        <v>108</v>
-      </c>
-      <c r="I26" s="2">
-        <v>2</v>
+      <c r="E26" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="27" spans="1:9">
       <c r="A27" t="s">
-        <v>61</v>
-      </c>
-      <c r="B27">
-        <v>5</v>
-      </c>
-      <c r="C27" s="1" t="s">
-        <v>4</v>
+        <v>156</v>
+      </c>
+      <c r="B27" s="5">
+        <v>7</v>
+      </c>
+      <c r="C27" t="s">
+        <v>6</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>5</v>
@@ -1278,63 +1392,70 @@
     </row>
     <row r="28" spans="1:9">
       <c r="A28" t="s">
-        <v>62</v>
-      </c>
-      <c r="B28">
-        <v>4</v>
+        <v>57</v>
+      </c>
+      <c r="B28" s="5">
+        <v>9</v>
       </c>
       <c r="C28" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
+      </c>
+      <c r="D28" t="s">
+        <v>42</v>
       </c>
       <c r="E28" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="29" spans="1:9">
       <c r="A29" t="s">
-        <v>63</v>
-      </c>
-      <c r="B29">
-        <v>3</v>
+        <v>157</v>
+      </c>
+      <c r="B29" s="5">
+        <v>8</v>
       </c>
       <c r="C29" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
+      </c>
+      <c r="D29" t="s">
+        <v>42</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>5</v>
+      </c>
+      <c r="F29" s="2">
+        <v>1000</v>
       </c>
     </row>
     <row r="30" spans="1:9">
       <c r="A30" t="s">
-        <v>64</v>
-      </c>
-      <c r="B30" s="7">
-        <f>B28</f>
-        <v>4</v>
-      </c>
-      <c r="C30" t="s">
-        <v>6</v>
+        <v>158</v>
+      </c>
+      <c r="B30" s="5">
+        <v>7</v>
+      </c>
+      <c r="C30" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D30" t="s">
+        <v>42</v>
       </c>
       <c r="E30" s="3" t="s">
-        <v>3</v>
-      </c>
-      <c r="F30" s="2">
-        <v>1000</v>
+        <v>5</v>
       </c>
     </row>
     <row r="31" spans="1:9">
       <c r="A31" t="s">
-        <v>65</v>
-      </c>
-      <c r="B31" s="7">
-        <f>B27</f>
-        <v>5</v>
+        <v>58</v>
+      </c>
+      <c r="B31" s="8">
+        <v>9</v>
       </c>
       <c r="C31" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D31" t="s">
-        <v>66</v>
+        <v>43</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>3</v>
@@ -1342,17 +1463,16 @@
     </row>
     <row r="32" spans="1:9">
       <c r="A32" t="s">
-        <v>67</v>
-      </c>
-      <c r="B32" s="7">
-        <f>B27</f>
-        <v>5</v>
+        <v>59</v>
+      </c>
+      <c r="B32" s="8">
+        <v>8</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D32" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>3</v>
@@ -1360,17 +1480,16 @@
     </row>
     <row r="33" spans="1:9">
       <c r="A33" t="s">
-        <v>69</v>
-      </c>
-      <c r="B33" s="7">
-        <f>B28</f>
-        <v>4</v>
+        <v>60</v>
+      </c>
+      <c r="B33" s="8">
+        <v>7</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>14</v>
       </c>
       <c r="D33" t="s">
-        <v>68</v>
+        <v>43</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>3</v>
@@ -1378,105 +1497,87 @@
     </row>
     <row r="34" spans="1:9">
       <c r="A34" t="s">
-        <v>70</v>
-      </c>
-      <c r="B34" s="7">
-        <f>B29</f>
-        <v>3</v>
-      </c>
-      <c r="C34" s="1" t="s">
-        <v>14</v>
-      </c>
-      <c r="D34" t="s">
-        <v>68</v>
-      </c>
-      <c r="E34" s="3" t="s">
-        <v>3</v>
+        <v>44</v>
+      </c>
+      <c r="B34" s="9">
+        <v>6</v>
+      </c>
+      <c r="C34" s="1"/>
+      <c r="G34" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H34" t="s">
+        <v>108</v>
+      </c>
+      <c r="I34" s="2">
+        <v>2</v>
       </c>
     </row>
     <row r="35" spans="1:9">
       <c r="A35" t="s">
-        <v>71</v>
-      </c>
-      <c r="B35">
-        <v>2</v>
-      </c>
-      <c r="C35" s="1"/>
-      <c r="G35" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H35" t="s">
-        <v>108</v>
-      </c>
-      <c r="I35" s="2">
-        <v>3</v>
+        <v>61</v>
+      </c>
+      <c r="B35" s="5">
+        <v>5</v>
+      </c>
+      <c r="C35" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="36" spans="1:9">
       <c r="A36" t="s">
-        <v>18</v>
-      </c>
-      <c r="B36" s="7">
-        <f>B39</f>
-        <v>27</v>
-      </c>
-      <c r="C36" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D36" s="5" t="s">
-        <v>15</v>
+        <v>62</v>
+      </c>
+      <c r="B36" s="5">
+        <v>4</v>
+      </c>
+      <c r="C36" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="E36" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="37" spans="1:9">
       <c r="A37" t="s">
-        <v>17</v>
-      </c>
-      <c r="B37" s="7">
-        <f>B38</f>
-        <v>25</v>
-      </c>
-      <c r="C37" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D37" s="5" t="s">
-        <v>10</v>
+        <v>63</v>
+      </c>
+      <c r="B37" s="5">
+        <v>3</v>
+      </c>
+      <c r="C37" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="E37" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="38" spans="1:9">
       <c r="A38" t="s">
-        <v>20</v>
-      </c>
-      <c r="B38">
-        <v>25</v>
-      </c>
-      <c r="C38" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D38" s="5" t="s">
-        <v>11</v>
+        <v>159</v>
+      </c>
+      <c r="B38" s="5">
+        <v>5</v>
+      </c>
+      <c r="C38" t="s">
+        <v>6</v>
       </c>
       <c r="E38" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="39" spans="1:9">
       <c r="A39" t="s">
-        <v>16</v>
-      </c>
-      <c r="B39">
-        <v>27</v>
-      </c>
-      <c r="C39" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D39" t="s">
-        <v>11</v>
+        <v>64</v>
+      </c>
+      <c r="B39" s="5">
+        <v>4</v>
+      </c>
+      <c r="C39" t="s">
+        <v>6</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>3</v>
@@ -1484,61 +1585,67 @@
     </row>
     <row r="40" spans="1:9">
       <c r="A40" t="s">
-        <v>19</v>
-      </c>
-      <c r="B40">
-        <v>29</v>
-      </c>
-      <c r="C40" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D40" t="s">
-        <v>11</v>
+        <v>160</v>
+      </c>
+      <c r="B40" s="5">
+        <v>3</v>
+      </c>
+      <c r="C40" t="s">
+        <v>6</v>
       </c>
       <c r="E40" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="41" spans="1:9">
       <c r="A41" t="s">
-        <v>21</v>
-      </c>
-      <c r="B41" s="7">
-        <f>B38</f>
-        <v>25</v>
+        <v>65</v>
+      </c>
+      <c r="B41" s="5">
+        <v>5</v>
       </c>
       <c r="C41" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
+      </c>
+      <c r="D41" t="s">
+        <v>66</v>
       </c>
       <c r="E41" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="42" spans="1:9">
       <c r="A42" t="s">
-        <v>22</v>
-      </c>
-      <c r="B42" s="7">
-        <f>B39</f>
-        <v>27</v>
+        <v>161</v>
+      </c>
+      <c r="B42" s="5">
+        <v>4</v>
       </c>
       <c r="C42" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
+      </c>
+      <c r="D42" t="s">
+        <v>66</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>5</v>
+      </c>
+      <c r="F42" s="2">
+        <v>1000</v>
       </c>
     </row>
     <row r="43" spans="1:9">
       <c r="A43" t="s">
-        <v>23</v>
-      </c>
-      <c r="B43" s="7">
-        <f>B40</f>
-        <v>29</v>
+        <v>162</v>
+      </c>
+      <c r="B43" s="5">
+        <v>3</v>
       </c>
       <c r="C43" s="1" t="s">
-        <v>4</v>
+        <v>14</v>
+      </c>
+      <c r="D43" t="s">
+        <v>66</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>5</v>
@@ -1546,53 +1653,50 @@
     </row>
     <row r="44" spans="1:9">
       <c r="A44" t="s">
-        <v>26</v>
-      </c>
-      <c r="B44" s="6">
-        <v>62</v>
-      </c>
-      <c r="C44" s="1"/>
-      <c r="G44" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H44" t="s">
-        <v>27</v>
-      </c>
-      <c r="I44" s="2" t="s">
-        <v>11</v>
+        <v>67</v>
+      </c>
+      <c r="B44" s="8">
+        <v>5</v>
+      </c>
+      <c r="C44" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D44" t="s">
+        <v>68</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="45" spans="1:9">
       <c r="A45" t="s">
-        <v>28</v>
-      </c>
-      <c r="B45" s="6">
-        <v>63</v>
-      </c>
-      <c r="C45" s="1"/>
-      <c r="G45" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H45" t="s">
-        <v>27</v>
-      </c>
-      <c r="I45" s="2" t="s">
-        <v>10</v>
+        <v>69</v>
+      </c>
+      <c r="B45" s="8">
+        <v>4</v>
+      </c>
+      <c r="C45" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D45" t="s">
+        <v>68</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="46" spans="1:9">
       <c r="A46" t="s">
-        <v>72</v>
-      </c>
-      <c r="B46" s="7">
-        <f>B49</f>
-        <v>33</v>
-      </c>
-      <c r="C46" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D46" s="5" t="s">
-        <v>73</v>
+        <v>70</v>
+      </c>
+      <c r="B46" s="8">
+        <v>3</v>
+      </c>
+      <c r="C46" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="D46" t="s">
+        <v>68</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>3</v>
@@ -1600,51 +1704,51 @@
     </row>
     <row r="47" spans="1:9">
       <c r="A47" t="s">
-        <v>74</v>
-      </c>
-      <c r="B47" s="7">
-        <f>B48</f>
-        <v>31</v>
-      </c>
-      <c r="C47" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D47" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="E47" s="3" t="s">
+        <v>71</v>
+      </c>
+      <c r="B47" s="9">
+        <v>2</v>
+      </c>
+      <c r="C47" s="1"/>
+      <c r="G47" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H47" t="s">
+        <v>108</v>
+      </c>
+      <c r="I47" s="2">
         <v>3</v>
       </c>
     </row>
     <row r="48" spans="1:9">
       <c r="A48" t="s">
-        <v>75</v>
-      </c>
-      <c r="B48">
-        <v>31</v>
-      </c>
-      <c r="C48" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D48" s="5" t="s">
-        <v>43</v>
+        <v>128</v>
+      </c>
+      <c r="B48" s="5">
+        <v>25</v>
+      </c>
+      <c r="C48" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D48" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="E48" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="49" spans="1:9">
       <c r="A49" t="s">
-        <v>76</v>
-      </c>
-      <c r="B49">
-        <v>33</v>
-      </c>
-      <c r="C49" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D49" t="s">
-        <v>43</v>
+        <v>18</v>
+      </c>
+      <c r="B49" s="5">
+        <v>27</v>
+      </c>
+      <c r="C49" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D49" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>3</v>
@@ -1652,46 +1756,50 @@
     </row>
     <row r="50" spans="1:9">
       <c r="A50" t="s">
-        <v>77</v>
-      </c>
-      <c r="B50">
-        <v>35</v>
-      </c>
-      <c r="C50" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D50" t="s">
-        <v>43</v>
+        <v>129</v>
+      </c>
+      <c r="B50" s="5">
+        <v>29</v>
+      </c>
+      <c r="C50" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D50" s="7" t="s">
+        <v>15</v>
       </c>
       <c r="E50" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="51" spans="1:9">
       <c r="A51" t="s">
-        <v>78</v>
-      </c>
-      <c r="B51" s="7">
-        <f>B48</f>
-        <v>31</v>
-      </c>
-      <c r="C51" s="1" t="s">
-        <v>4</v>
+        <v>17</v>
+      </c>
+      <c r="B51" s="5">
+        <v>25</v>
+      </c>
+      <c r="C51" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D51" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="E51" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="52" spans="1:9">
       <c r="A52" t="s">
-        <v>79</v>
-      </c>
-      <c r="B52" s="7">
-        <f>B49</f>
-        <v>33</v>
-      </c>
-      <c r="C52" s="1" t="s">
-        <v>4</v>
+        <v>120</v>
+      </c>
+      <c r="B52" s="5">
+        <v>27</v>
+      </c>
+      <c r="C52" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D52" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>5</v>
@@ -1699,14 +1807,16 @@
     </row>
     <row r="53" spans="1:9">
       <c r="A53" t="s">
-        <v>80</v>
-      </c>
-      <c r="B53" s="7">
-        <f>B50</f>
-        <v>35</v>
-      </c>
-      <c r="C53" s="1" t="s">
-        <v>4</v>
+        <v>130</v>
+      </c>
+      <c r="B53" s="5">
+        <v>29</v>
+      </c>
+      <c r="C53" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D53" s="7" t="s">
+        <v>10</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>5</v>
@@ -1714,53 +1824,50 @@
     </row>
     <row r="54" spans="1:9">
       <c r="A54" t="s">
-        <v>81</v>
-      </c>
-      <c r="B54" s="6">
-        <v>60</v>
-      </c>
-      <c r="C54" s="1"/>
-      <c r="G54" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H54" t="s">
-        <v>27</v>
-      </c>
-      <c r="I54" s="2" t="s">
-        <v>43</v>
+        <v>20</v>
+      </c>
+      <c r="B54">
+        <v>25</v>
+      </c>
+      <c r="C54" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D54" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="E54" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="55" spans="1:9">
       <c r="A55" t="s">
-        <v>82</v>
-      </c>
-      <c r="B55" s="6">
-        <v>61</v>
-      </c>
-      <c r="C55" s="1"/>
-      <c r="G55" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H55" t="s">
+        <v>16</v>
+      </c>
+      <c r="B55">
         <v>27</v>
       </c>
-      <c r="I55" s="2" t="s">
-        <v>42</v>
+      <c r="C55" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D55" t="s">
+        <v>11</v>
+      </c>
+      <c r="E55" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="56" spans="1:9">
       <c r="A56" t="s">
-        <v>83</v>
-      </c>
-      <c r="B56" s="7">
-        <f>B59</f>
-        <v>39</v>
-      </c>
-      <c r="C56" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D56" s="5" t="s">
-        <v>84</v>
+        <v>19</v>
+      </c>
+      <c r="B56">
+        <v>29</v>
+      </c>
+      <c r="C56" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D56" t="s">
+        <v>11</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>3</v>
@@ -1768,98 +1875,94 @@
     </row>
     <row r="57" spans="1:9">
       <c r="A57" t="s">
-        <v>85</v>
-      </c>
-      <c r="B57" s="7">
-        <f>B58</f>
-        <v>37</v>
-      </c>
-      <c r="C57" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D57" s="5" t="s">
-        <v>66</v>
+        <v>21</v>
+      </c>
+      <c r="B57" s="5">
+        <v>25</v>
+      </c>
+      <c r="C57" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="E57" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="58" spans="1:9">
       <c r="A58" t="s">
-        <v>86</v>
-      </c>
-      <c r="B58">
-        <v>37</v>
-      </c>
-      <c r="C58" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D58" s="5" t="s">
-        <v>68</v>
+        <v>22</v>
+      </c>
+      <c r="B58" s="5">
+        <v>27</v>
+      </c>
+      <c r="C58" s="1" t="s">
+        <v>4</v>
       </c>
       <c r="E58" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="59" spans="1:9">
       <c r="A59" t="s">
-        <v>87</v>
-      </c>
-      <c r="B59">
-        <v>39</v>
+        <v>23</v>
+      </c>
+      <c r="B59" s="5">
+        <v>29</v>
       </c>
       <c r="C59" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D59" t="s">
-        <v>68</v>
+        <v>4</v>
       </c>
       <c r="E59" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="60" spans="1:9">
       <c r="A60" t="s">
-        <v>88</v>
-      </c>
-      <c r="B60">
-        <v>41</v>
-      </c>
-      <c r="C60" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D60" t="s">
-        <v>68</v>
-      </c>
-      <c r="E60" s="3" t="s">
-        <v>3</v>
+        <v>26</v>
+      </c>
+      <c r="B60" s="4">
+        <v>62</v>
+      </c>
+      <c r="C60" s="1"/>
+      <c r="G60" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H60" t="s">
+        <v>27</v>
+      </c>
+      <c r="I60" s="2" t="s">
+        <v>11</v>
       </c>
     </row>
     <row r="61" spans="1:9">
       <c r="A61" t="s">
-        <v>89</v>
-      </c>
-      <c r="B61" s="7">
-        <f>B58</f>
-        <v>37</v>
-      </c>
-      <c r="C61" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="E61" s="3" t="s">
-        <v>5</v>
+        <v>28</v>
+      </c>
+      <c r="B61" s="4">
+        <v>63</v>
+      </c>
+      <c r="C61" s="1"/>
+      <c r="G61" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H61" t="s">
+        <v>27</v>
+      </c>
+      <c r="I61" s="2" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="62" spans="1:9">
       <c r="A62" t="s">
-        <v>90</v>
-      </c>
-      <c r="B62" s="7">
-        <f>B59</f>
-        <v>39</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>4</v>
+        <v>126</v>
+      </c>
+      <c r="B62" s="5">
+        <v>31</v>
+      </c>
+      <c r="C62" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D62" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>5</v>
@@ -1867,103 +1970,101 @@
     </row>
     <row r="63" spans="1:9">
       <c r="A63" t="s">
-        <v>91</v>
-      </c>
-      <c r="B63" s="7">
-        <f>B60</f>
-        <v>41</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>4</v>
+        <v>72</v>
+      </c>
+      <c r="B63" s="5">
+        <v>33</v>
+      </c>
+      <c r="C63" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D63" s="7" t="s">
+        <v>73</v>
       </c>
       <c r="E63" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="64" spans="1:9">
       <c r="A64" t="s">
-        <v>92</v>
-      </c>
-      <c r="B64" s="6">
-        <v>58</v>
-      </c>
-      <c r="C64" s="1"/>
-      <c r="G64" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H64" t="s">
-        <v>27</v>
-      </c>
-      <c r="I64" s="2" t="s">
-        <v>68</v>
+        <v>127</v>
+      </c>
+      <c r="B64" s="5">
+        <v>35</v>
+      </c>
+      <c r="C64" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D64" s="7" t="s">
+        <v>73</v>
+      </c>
+      <c r="E64" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="65" spans="1:9">
       <c r="A65" t="s">
-        <v>93</v>
-      </c>
-      <c r="B65" s="6">
-        <v>59</v>
-      </c>
-      <c r="C65" s="1"/>
-      <c r="G65" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H65" t="s">
-        <v>27</v>
-      </c>
-      <c r="I65" s="2" t="s">
-        <v>66</v>
+        <v>74</v>
+      </c>
+      <c r="B65" s="5">
+        <v>31</v>
+      </c>
+      <c r="C65" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D65" s="7" t="s">
+        <v>42</v>
+      </c>
+      <c r="E65" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="66" spans="1:9">
       <c r="A66" t="s">
-        <v>94</v>
-      </c>
-      <c r="B66" s="7">
-        <f>B69</f>
-        <v>45</v>
-      </c>
-      <c r="C66" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D66" s="5" t="s">
-        <v>95</v>
+        <v>121</v>
+      </c>
+      <c r="B66" s="5">
+        <v>33</v>
+      </c>
+      <c r="C66" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D66" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="E66" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="67" spans="1:9">
       <c r="A67" t="s">
-        <v>96</v>
-      </c>
-      <c r="B67" s="7">
-        <f>B68</f>
-        <v>43</v>
-      </c>
-      <c r="C67" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D67" s="5" t="s">
-        <v>97</v>
+        <v>125</v>
+      </c>
+      <c r="B67" s="5">
+        <v>35</v>
+      </c>
+      <c r="C67" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D67" s="7" t="s">
+        <v>42</v>
       </c>
       <c r="E67" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="68" spans="1:9">
       <c r="A68" t="s">
-        <v>98</v>
+        <v>75</v>
       </c>
       <c r="B68">
+        <v>31</v>
+      </c>
+      <c r="C68" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D68" s="7" t="s">
         <v>43</v>
-      </c>
-      <c r="C68" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D68" s="5" t="s">
-        <v>99</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>3</v>
@@ -1971,16 +2072,16 @@
     </row>
     <row r="69" spans="1:9">
       <c r="A69" t="s">
-        <v>100</v>
+        <v>76</v>
       </c>
       <c r="B69">
-        <v>45</v>
+        <v>33</v>
       </c>
       <c r="C69" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D69" t="s">
-        <v>99</v>
+        <v>43</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>3</v>
@@ -1988,16 +2089,16 @@
     </row>
     <row r="70" spans="1:9">
       <c r="A70" t="s">
-        <v>101</v>
+        <v>77</v>
       </c>
       <c r="B70">
-        <v>47</v>
+        <v>35</v>
       </c>
       <c r="C70" s="1" t="s">
         <v>24</v>
       </c>
       <c r="D70" t="s">
-        <v>99</v>
+        <v>43</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>3</v>
@@ -2005,11 +2106,10 @@
     </row>
     <row r="71" spans="1:9">
       <c r="A71" t="s">
-        <v>102</v>
-      </c>
-      <c r="B71" s="7">
-        <f>B68</f>
-        <v>43</v>
+        <v>78</v>
+      </c>
+      <c r="B71" s="5">
+        <v>31</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>4</v>
@@ -2020,11 +2120,10 @@
     </row>
     <row r="72" spans="1:9">
       <c r="A72" t="s">
-        <v>103</v>
-      </c>
-      <c r="B72" s="7">
-        <f>B69</f>
-        <v>45</v>
+        <v>79</v>
+      </c>
+      <c r="B72" s="5">
+        <v>33</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>4</v>
@@ -2035,11 +2134,10 @@
     </row>
     <row r="73" spans="1:9">
       <c r="A73" t="s">
-        <v>104</v>
-      </c>
-      <c r="B73" s="7">
-        <f>B70</f>
-        <v>47</v>
+        <v>80</v>
+      </c>
+      <c r="B73" s="5">
+        <v>35</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>4</v>
@@ -2050,10 +2148,10 @@
     </row>
     <row r="74" spans="1:9">
       <c r="A74" t="s">
-        <v>105</v>
-      </c>
-      <c r="B74" s="6">
-        <v>56</v>
+        <v>81</v>
+      </c>
+      <c r="B74" s="4">
+        <v>60</v>
       </c>
       <c r="C74" s="1"/>
       <c r="G74" s="2" t="s">
@@ -2063,15 +2161,15 @@
         <v>27</v>
       </c>
       <c r="I74" s="2" t="s">
-        <v>99</v>
+        <v>43</v>
       </c>
     </row>
     <row r="75" spans="1:9">
       <c r="A75" t="s">
-        <v>106</v>
-      </c>
-      <c r="B75" s="6">
-        <v>57</v>
+        <v>82</v>
+      </c>
+      <c r="B75" s="4">
+        <v>61</v>
       </c>
       <c r="C75" s="1"/>
       <c r="G75" s="2" t="s">
@@ -2081,40 +2179,38 @@
         <v>27</v>
       </c>
       <c r="I75" s="2" t="s">
-        <v>97</v>
+        <v>42</v>
       </c>
     </row>
     <row r="76" spans="1:9">
       <c r="A76" t="s">
-        <v>94</v>
-      </c>
-      <c r="B76" s="7">
-        <f>B79</f>
-        <v>51</v>
-      </c>
-      <c r="C76" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D76" s="5" t="s">
-        <v>95</v>
+        <v>131</v>
+      </c>
+      <c r="B76" s="5">
+        <v>37</v>
+      </c>
+      <c r="C76" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D76" s="7" t="s">
+        <v>84</v>
       </c>
       <c r="E76" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="77" spans="1:9">
       <c r="A77" t="s">
-        <v>96</v>
-      </c>
-      <c r="B77" s="7">
-        <f>B78</f>
-        <v>49</v>
-      </c>
-      <c r="C77" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D77" s="5" t="s">
-        <v>97</v>
+        <v>83</v>
+      </c>
+      <c r="B77" s="5">
+        <v>39</v>
+      </c>
+      <c r="C77" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D77" s="7" t="s">
+        <v>84</v>
       </c>
       <c r="E77" s="3" t="s">
         <v>3</v>
@@ -2122,33 +2218,33 @@
     </row>
     <row r="78" spans="1:9">
       <c r="A78" t="s">
-        <v>98</v>
-      </c>
-      <c r="B78">
-        <v>49</v>
-      </c>
-      <c r="C78" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="D78" s="5" t="s">
-        <v>99</v>
+        <v>132</v>
+      </c>
+      <c r="B78" s="5">
+        <v>41</v>
+      </c>
+      <c r="C78" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D78" s="7" t="s">
+        <v>84</v>
       </c>
       <c r="E78" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="79" spans="1:9">
       <c r="A79" t="s">
-        <v>100</v>
-      </c>
-      <c r="B79">
-        <v>51</v>
-      </c>
-      <c r="C79" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D79" t="s">
-        <v>99</v>
+        <v>85</v>
+      </c>
+      <c r="B79" s="5">
+        <v>37</v>
+      </c>
+      <c r="C79" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D79" s="7" t="s">
+        <v>66</v>
       </c>
       <c r="E79" s="3" t="s">
         <v>3</v>
@@ -2156,31 +2252,33 @@
     </row>
     <row r="80" spans="1:9">
       <c r="A80" t="s">
-        <v>101</v>
-      </c>
-      <c r="B80">
-        <v>53</v>
-      </c>
-      <c r="C80" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D80" t="s">
-        <v>99</v>
+        <v>122</v>
+      </c>
+      <c r="B80" s="5">
+        <v>39</v>
+      </c>
+      <c r="C80" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D80" s="7" t="s">
+        <v>66</v>
       </c>
       <c r="E80" s="3" t="s">
-        <v>3</v>
+        <v>5</v>
       </c>
     </row>
     <row r="81" spans="1:9">
       <c r="A81" t="s">
-        <v>102</v>
-      </c>
-      <c r="B81" s="7">
-        <f>B78</f>
-        <v>49</v>
-      </c>
-      <c r="C81" s="1" t="s">
-        <v>4</v>
+        <v>133</v>
+      </c>
+      <c r="B81" s="5">
+        <v>41</v>
+      </c>
+      <c r="C81" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D81" s="7" t="s">
+        <v>66</v>
       </c>
       <c r="E81" s="3" t="s">
         <v>5</v>
@@ -2188,133 +2286,658 @@
     </row>
     <row r="82" spans="1:9">
       <c r="A82" t="s">
-        <v>103</v>
-      </c>
-      <c r="B82" s="7">
-        <f>B79</f>
-        <v>51</v>
-      </c>
-      <c r="C82" s="1" t="s">
-        <v>4</v>
+        <v>86</v>
+      </c>
+      <c r="B82">
+        <v>37</v>
+      </c>
+      <c r="C82" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D82" s="7" t="s">
+        <v>68</v>
       </c>
       <c r="E82" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="83" spans="1:9">
       <c r="A83" t="s">
-        <v>104</v>
-      </c>
-      <c r="B83" s="7">
-        <f>B80</f>
-        <v>53</v>
+        <v>87</v>
+      </c>
+      <c r="B83">
+        <v>39</v>
       </c>
       <c r="C83" s="1" t="s">
-        <v>4</v>
+        <v>24</v>
+      </c>
+      <c r="D83" t="s">
+        <v>68</v>
       </c>
       <c r="E83" s="3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="84" spans="1:9">
       <c r="A84" t="s">
-        <v>105</v>
-      </c>
-      <c r="B84" s="6">
-        <v>54</v>
-      </c>
-      <c r="C84" s="1"/>
-      <c r="G84" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H84" t="s">
-        <v>27</v>
-      </c>
-      <c r="I84" s="2" t="s">
-        <v>118</v>
+        <v>88</v>
+      </c>
+      <c r="B84">
+        <v>41</v>
+      </c>
+      <c r="C84" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D84" t="s">
+        <v>68</v>
+      </c>
+      <c r="E84" s="3" t="s">
+        <v>3</v>
       </c>
     </row>
     <row r="85" spans="1:9">
       <c r="A85" t="s">
-        <v>106</v>
-      </c>
-      <c r="B85" s="6">
-        <v>55</v>
-      </c>
-      <c r="C85" s="1"/>
-      <c r="G85" s="2" t="s">
-        <v>3</v>
-      </c>
-      <c r="H85" t="s">
-        <v>27</v>
-      </c>
-      <c r="I85" s="2" t="s">
-        <v>119</v>
+        <v>89</v>
+      </c>
+      <c r="B85" s="5">
+        <v>37</v>
+      </c>
+      <c r="C85" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E85" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="86" spans="1:9">
       <c r="A86" t="s">
-        <v>117</v>
-      </c>
-      <c r="B86">
-        <v>64</v>
+        <v>90</v>
+      </c>
+      <c r="B86" s="5">
+        <v>39</v>
       </c>
       <c r="C86" s="1" t="s">
-        <v>116</v>
+        <v>4</v>
+      </c>
+      <c r="E86" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="87" spans="1:9">
       <c r="A87" t="s">
-        <v>111</v>
-      </c>
-      <c r="B87">
-        <v>65</v>
+        <v>91</v>
+      </c>
+      <c r="B87" s="5">
+        <v>41</v>
       </c>
       <c r="C87" s="1" t="s">
-        <v>116</v>
+        <v>4</v>
+      </c>
+      <c r="E87" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="88" spans="1:9">
       <c r="A88" t="s">
-        <v>112</v>
-      </c>
-      <c r="B88">
-        <v>66</v>
-      </c>
-      <c r="C88" s="1" t="s">
-        <v>116</v>
+        <v>92</v>
+      </c>
+      <c r="B88" s="4">
+        <v>58</v>
+      </c>
+      <c r="C88" s="1"/>
+      <c r="G88" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H88" t="s">
+        <v>27</v>
+      </c>
+      <c r="I88" s="2" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="89" spans="1:9">
       <c r="A89" t="s">
-        <v>113</v>
-      </c>
-      <c r="B89">
-        <v>67</v>
-      </c>
-      <c r="C89" s="1" t="s">
-        <v>116</v>
+        <v>93</v>
+      </c>
+      <c r="B89" s="4">
+        <v>59</v>
+      </c>
+      <c r="C89" s="1"/>
+      <c r="G89" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H89" t="s">
+        <v>27</v>
+      </c>
+      <c r="I89" s="2" t="s">
+        <v>66</v>
       </c>
     </row>
     <row r="90" spans="1:9">
       <c r="A90" t="s">
-        <v>114</v>
-      </c>
-      <c r="B90">
-        <v>68</v>
-      </c>
-      <c r="C90" s="1" t="s">
-        <v>116</v>
+        <v>134</v>
+      </c>
+      <c r="B90" s="5">
+        <v>45</v>
+      </c>
+      <c r="C90" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D90" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E90" s="3" t="s">
+        <v>5</v>
       </c>
     </row>
     <row r="91" spans="1:9">
       <c r="A91" t="s">
+        <v>94</v>
+      </c>
+      <c r="B91" s="5">
+        <v>43</v>
+      </c>
+      <c r="C91" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D91" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E91" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="92" spans="1:9">
+      <c r="A92" t="s">
+        <v>135</v>
+      </c>
+      <c r="B92" s="5">
+        <v>45</v>
+      </c>
+      <c r="C92" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D92" s="7" t="s">
+        <v>95</v>
+      </c>
+      <c r="E92" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9">
+      <c r="A93" t="s">
+        <v>96</v>
+      </c>
+      <c r="B93" s="5">
+        <v>45</v>
+      </c>
+      <c r="C93" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D93" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="E93" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9">
+      <c r="A94" t="s">
+        <v>123</v>
+      </c>
+      <c r="B94" s="5">
+        <v>43</v>
+      </c>
+      <c r="C94" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D94" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="E94" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9">
+      <c r="A95" t="s">
+        <v>136</v>
+      </c>
+      <c r="B95" s="5">
+        <v>45</v>
+      </c>
+      <c r="C95" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D95" s="7" t="s">
+        <v>97</v>
+      </c>
+      <c r="E95" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="96" spans="1:9">
+      <c r="A96" t="s">
+        <v>98</v>
+      </c>
+      <c r="B96">
+        <v>43</v>
+      </c>
+      <c r="C96" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D96" s="7" t="s">
+        <v>99</v>
+      </c>
+      <c r="E96" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="97" spans="1:9">
+      <c r="A97" t="s">
+        <v>100</v>
+      </c>
+      <c r="B97">
+        <v>45</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D97" t="s">
+        <v>99</v>
+      </c>
+      <c r="E97" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="98" spans="1:9">
+      <c r="A98" t="s">
+        <v>101</v>
+      </c>
+      <c r="B98">
+        <v>47</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D98" t="s">
+        <v>99</v>
+      </c>
+      <c r="E98" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="99" spans="1:9">
+      <c r="A99" t="s">
+        <v>102</v>
+      </c>
+      <c r="B99" s="5">
+        <v>43</v>
+      </c>
+      <c r="C99" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E99" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="100" spans="1:9">
+      <c r="A100" t="s">
+        <v>103</v>
+      </c>
+      <c r="B100" s="5">
+        <v>45</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E100" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="101" spans="1:9">
+      <c r="A101" t="s">
+        <v>104</v>
+      </c>
+      <c r="B101" s="5">
+        <v>47</v>
+      </c>
+      <c r="C101" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E101" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="102" spans="1:9">
+      <c r="A102" t="s">
+        <v>105</v>
+      </c>
+      <c r="B102" s="4">
+        <v>56</v>
+      </c>
+      <c r="C102" s="1"/>
+      <c r="G102" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H102" t="s">
+        <v>27</v>
+      </c>
+      <c r="I102" s="2" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="103" spans="1:9">
+      <c r="A103" t="s">
+        <v>106</v>
+      </c>
+      <c r="B103" s="4">
+        <v>57</v>
+      </c>
+      <c r="C103" s="1"/>
+      <c r="G103" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H103" t="s">
+        <v>27</v>
+      </c>
+      <c r="I103" s="2" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="104" spans="1:9">
+      <c r="A104" t="s">
+        <v>137</v>
+      </c>
+      <c r="B104" s="5">
+        <v>49</v>
+      </c>
+      <c r="C104" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D104" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="E104" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="105" spans="1:9">
+      <c r="A105" t="s">
+        <v>139</v>
+      </c>
+      <c r="B105" s="5">
+        <v>51</v>
+      </c>
+      <c r="C105" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D105" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="E105" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="106" spans="1:9">
+      <c r="A106" t="s">
+        <v>140</v>
+      </c>
+      <c r="B106" s="5">
+        <v>53</v>
+      </c>
+      <c r="C106" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D106" s="7" t="s">
+        <v>138</v>
+      </c>
+      <c r="E106" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="107" spans="1:9">
+      <c r="A107" t="s">
+        <v>141</v>
+      </c>
+      <c r="B107" s="5">
+        <v>49</v>
+      </c>
+      <c r="C107" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D107" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="E107" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="108" spans="1:9">
+      <c r="A108" t="s">
+        <v>124</v>
+      </c>
+      <c r="B108" s="5">
+        <v>51</v>
+      </c>
+      <c r="C108" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D108" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="E108" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="109" spans="1:9">
+      <c r="A109" t="s">
+        <v>142</v>
+      </c>
+      <c r="B109" s="5">
+        <v>53</v>
+      </c>
+      <c r="C109" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D109" s="7" t="s">
+        <v>119</v>
+      </c>
+      <c r="E109" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="110" spans="1:9">
+      <c r="A110" t="s">
+        <v>143</v>
+      </c>
+      <c r="B110">
+        <v>49</v>
+      </c>
+      <c r="C110" s="6" t="s">
+        <v>24</v>
+      </c>
+      <c r="D110" s="7" t="s">
+        <v>118</v>
+      </c>
+      <c r="E110" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="111" spans="1:9">
+      <c r="A111" t="s">
+        <v>144</v>
+      </c>
+      <c r="B111">
+        <v>51</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D111" t="s">
+        <v>118</v>
+      </c>
+      <c r="E111" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:9">
+      <c r="A112" t="s">
+        <v>145</v>
+      </c>
+      <c r="B112">
+        <v>53</v>
+      </c>
+      <c r="C112" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="D112" t="s">
+        <v>118</v>
+      </c>
+      <c r="E112" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="113" spans="1:9">
+      <c r="A113" t="s">
+        <v>146</v>
+      </c>
+      <c r="B113" s="5">
+        <v>49</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E113" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="114" spans="1:9">
+      <c r="A114" t="s">
+        <v>147</v>
+      </c>
+      <c r="B114" s="5">
+        <v>51</v>
+      </c>
+      <c r="C114" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E114" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="115" spans="1:9">
+      <c r="A115" t="s">
+        <v>148</v>
+      </c>
+      <c r="B115" s="5">
+        <v>53</v>
+      </c>
+      <c r="C115" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E115" s="3" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="116" spans="1:9">
+      <c r="A116" t="s">
+        <v>149</v>
+      </c>
+      <c r="B116" s="4">
+        <v>54</v>
+      </c>
+      <c r="C116" s="1"/>
+      <c r="G116" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H116" t="s">
+        <v>27</v>
+      </c>
+      <c r="I116" s="2" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="117" spans="1:9">
+      <c r="A117" t="s">
+        <v>150</v>
+      </c>
+      <c r="B117" s="4">
+        <v>55</v>
+      </c>
+      <c r="C117" s="1"/>
+      <c r="G117" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="H117" t="s">
+        <v>27</v>
+      </c>
+      <c r="I117" s="2" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="118" spans="1:9">
+      <c r="A118" t="s">
+        <v>117</v>
+      </c>
+      <c r="B118">
+        <v>64</v>
+      </c>
+      <c r="C118" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="119" spans="1:9">
+      <c r="A119" t="s">
+        <v>111</v>
+      </c>
+      <c r="B119">
+        <v>65</v>
+      </c>
+      <c r="C119" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="120" spans="1:9">
+      <c r="A120" t="s">
+        <v>112</v>
+      </c>
+      <c r="B120">
+        <v>66</v>
+      </c>
+      <c r="C120" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="121" spans="1:9">
+      <c r="A121" t="s">
+        <v>113</v>
+      </c>
+      <c r="B121">
+        <v>67</v>
+      </c>
+      <c r="C121" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="122" spans="1:9">
+      <c r="A122" t="s">
+        <v>114</v>
+      </c>
+      <c r="B122">
+        <v>68</v>
+      </c>
+      <c r="C122" s="1" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="123" spans="1:9">
+      <c r="A123" t="s">
         <v>115</v>
       </c>
-      <c r="B91">
+      <c r="B123">
         <v>69</v>
       </c>
-      <c r="C91" s="1" t="s">
+      <c r="C123" s="1" t="s">
         <v>116</v>
       </c>
     </row>

</xml_diff>